<commit_message>
Added description property for project; show more/less button for description in project detaisl view is set to work properly
</commit_message>
<xml_diff>
--- a/enterprice_task_list.xlsx
+++ b/enterprice_task_list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9528"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>projects tab</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>add photo property of user</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -113,12 +116,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -133,11 +142,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,21 +428,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="77" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -446,7 +456,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -460,7 +470,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -474,7 +484,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -488,7 +498,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -499,32 +509,38 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="F6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
occupation model created; users can choose between created occupations at register and this will define their initial rate while changing the rate of an occupation later will also affect all users with this occupation
</commit_message>
<xml_diff>
--- a/enterprice_task_list.xlsx
+++ b/enterprice_task_list.xlsx
@@ -491,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Actual expenses can be entered; rates for individuals can be changed
</commit_message>
<xml_diff>
--- a/enterprice_task_list.xlsx
+++ b/enterprice_task_list.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>projects tab</t>
   </si>
@@ -492,7 +492,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,15 +621,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="2" t="s">
         <v>18</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -640,7 +643,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>

</xml_diff>